<commit_message>
Implemented most of ftlua::push and ftlua::Keys
</commit_message>
<xml_diff>
--- a/modules/ftlua/callOverloads.xlsx
+++ b/modules/ftlua/callOverloads.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="1120" windowWidth="30500" windowHeight="26660" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="30500" windowHeight="26660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="94">
   <si>
     <t xml:space="preserve">PUSHED </t>
   </si>
@@ -50,18 +50,9 @@
     <t>CPP PARAMS</t>
   </si>
   <si>
-    <t>T const &amp;funTabKey</t>
-  </si>
-  <si>
     <t>nparams on the stack</t>
   </si>
   <si>
-    <t>T const &amp;funGlobalKey</t>
-  </si>
-  <si>
-    <t>T const &amp;tabGlobalKey</t>
-  </si>
-  <si>
     <t>Table repushed</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
     <t>callTMethod</t>
   </si>
   <si>
-    <t>callGTabTFun</t>
-  </si>
-  <si>
     <t>callGTabTMethod</t>
   </si>
   <si>
@@ -309,6 +297,15 @@
   </si>
   <si>
     <t>ftlua::Keys&lt;Any&gt;</t>
+  </si>
+  <si>
+    <t>ftlua::Keys&lt;ARGS...&gt; const &amp;funTabKeys</t>
+  </si>
+  <si>
+    <t>ftlua::Keys&lt;ARGS...&gt; const &amp;methodTabKeys</t>
+  </si>
+  <si>
+    <t>ftlua::Keys&lt;ARGS...&gt; const &amp;tabGlobalKeys</t>
   </si>
 </sst>
 </file>
@@ -667,14 +664,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="144" zoomScaleNormal="144" zoomScalePageLayoutView="144" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" zoomScale="144" zoomScaleNormal="144" zoomScalePageLayoutView="144" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="33.5" customWidth="1"/>
     <col min="4" max="5" width="21.33203125" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -692,39 +689,39 @@
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -738,109 +735,92 @@
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
       <c r="K7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" t="s">
         <v>35</v>
       </c>
-      <c r="J8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J9" t="s">
+      <c r="K9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" t="s">
         <v>39</v>
-      </c>
-      <c r="K9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -848,266 +828,266 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" t="s">
         <v>36</v>
       </c>
-      <c r="J13" t="s">
-        <v>40</v>
-      </c>
       <c r="K13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J20" t="s">
+        <v>53</v>
+      </c>
+      <c r="K20" t="s">
         <v>57</v>
-      </c>
-      <c r="K20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s">
         <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="J25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="J28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K28" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J29" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G31" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1115,10 +1095,10 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1126,79 +1106,79 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E34" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G36" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G39" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F40" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E41" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>